<commit_message>
Added stats of original Mark V
(non hypertuned version)
</commit_message>
<xml_diff>
--- a/Test Models/Nico/mark_V_stats.xlsx
+++ b/Test Models/Nico/mark_V_stats.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Desktop\Nicolas\Chalmers\054307-ARTIFICIAL_NEURAL_NETWORKS_AND_DEEP_LEARNING\Challenges\CompetitionOne\MarkV-stats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Desktop\Nicolas\Chalmers\054307-ARTIFICIAL_NEURAL_NETWORKS_AND_DEEP_LEARNING\Challenges\CompetitionOne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49D748F-D81E-4740-AB16-BCEAB1679153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3885CCD1-E79E-4CD1-8A0E-B5BF86B8AD9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>No.</t>
   </si>
@@ -120,13 +120,22 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>org</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>(0, 0)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +147,18 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFB5CEA8"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -175,12 +196,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -485,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -662,7 +693,7 @@
         <v>19</v>
       </c>
       <c r="K4" s="2">
-        <v>0.19711747765541071</v>
+        <v>0.19711747765541099</v>
       </c>
       <c r="L4" s="2">
         <v>0.92400002479553223</v>
@@ -875,6 +906,50 @@
       <c r="M9" s="2" t="s">
         <v>28</v>
       </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10">
+        <v>64</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0.21590000000000001</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="M10" s="4">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>